<commit_message>
removed filter button from admin-activities lists , added import template sample for region , city , errand categories-errands-types , zones , lookup fr reset of lists , added missing apis for import in locations , fixed label renaming in merchant form in category input
</commit_message>
<xml_diff>
--- a/src/assets/samples/ImportMerchantSample.xlsx
+++ b/src/assets/samples/ImportMerchantSample.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\personal\Softweaves-Frontend\src\assets\samples\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A5F71A-D739-479F-B2C2-A40AE3451F0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="5370" yWindow="1170" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,19 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>NameEn</t>
+  </si>
+  <si>
+    <t>NameAr</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -330,13 +347,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added template for merchant and terminal list in import
</commit_message>
<xml_diff>
--- a/src/assets/samples/ImportMerchantSample.xlsx
+++ b/src/assets/samples/ImportMerchantSample.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Afaqy\Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B152EBC2-B817-4ACA-A61D-B855FC9907CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{01F2EFFB-8856-46DA-B1D5-BEF19203C2BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -18,8 +24,46 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>MerchantId</t>
+  </si>
+  <si>
+    <t>NameEn</t>
+  </si>
+  <si>
+    <t>NameAr</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>CategoryId</t>
+  </si>
+  <si>
+    <t>Phonenumber</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Landmark</t>
+  </si>
+  <si>
+    <t>ZoneId</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -49,8 +93,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -85,7 +130,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -97,7 +142,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -144,6 +189,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -179,6 +241,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -330,13 +409,64 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ECF4BFC-3E68-4313-9447-328D3C2E1C8E}">
+  <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:K2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
hide filter in locations lists
</commit_message>
<xml_diff>
--- a/src/assets/samples/ImportMerchantSample.xlsx
+++ b/src/assets/samples/ImportMerchantSample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Afaqy\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Publish\OC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B152EBC2-B817-4ACA-A61D-B855FC9907CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37A1008A-49C2-4E17-8F92-EB0777D640AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{01F2EFFB-8856-46DA-B1D5-BEF19203C2BC}"/>
+    <workbookView xWindow="2010" yWindow="0" windowWidth="21975" windowHeight="20880" xr2:uid="{01F2EFFB-8856-46DA-B1D5-BEF19203C2BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>MerchantId</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>NameEn</t>
   </si>
@@ -39,9 +36,6 @@
     <t>Username</t>
   </si>
   <si>
-    <t>CategoryId</t>
-  </si>
-  <si>
     <t>Phonenumber</t>
   </si>
   <si>
@@ -57,7 +51,19 @@
     <t>Landmark</t>
   </si>
   <si>
-    <t>ZoneId</t>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Zone</t>
+  </si>
+  <si>
+    <t>Sales Agent</t>
+  </si>
+  <si>
+    <t>Service Agent</t>
+  </si>
+  <si>
+    <t>Merchant ID</t>
   </si>
 </sst>
 </file>
@@ -68,7 +74,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -410,60 +416,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ECF4BFC-3E68-4313-9447-328D3C2E1C8E}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:K2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" style="1"/>
+    <col min="12" max="12" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>